<commit_message>
new folders and class
</commit_message>
<xml_diff>
--- a/doc/workplan.xlsx
+++ b/doc/workplan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpelda\Documents\GitHub\memphis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpelda\Documents\GitHub\memphis\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -62,9 +62,6 @@
     <t>Upload Gis-Data Niedersachsen  (WGS 84, name: gis_road, gis_buildings, …, geopandas.GeoDataFrame()). Lukas about relevant data.</t>
   </si>
   <si>
-    <t>Upload Census  (EPSG 3035 -&gt; WGS 84, name: census, geopandas.GeoDataFrame()).</t>
-  </si>
-  <si>
     <t>Transform Gis-Data into graph (WGS 84, name: G, networkx.Graph()).</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>Allocate inhabitants of census 100 x 100 sqm with git_buildings['iPsqm']. Save it in  gis_buildings[“inhabitants“].</t>
+  </si>
+  <si>
+    <t>Upload Census  (name: census, geopandas.GeoDataFrame()).</t>
   </si>
 </sst>
 </file>
@@ -427,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -458,9 +458,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C3" s="6">
         <v>43153</v>
@@ -497,7 +497,7 @@
     </row>
     <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="6">
         <v>43160</v>
@@ -526,7 +526,7 @@
     </row>
     <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="6">
         <v>43170</v>
@@ -534,7 +534,7 @@
     </row>
     <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="6">
         <v>43170</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="20" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="6">
         <v>43174</v>
@@ -550,12 +550,12 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" s="6">
         <v>43179</v>

</xml_diff>